<commit_message>
I've added a scrap of table in XLSX
</commit_message>
<xml_diff>
--- a/Highly_likely_Table.xlsx
+++ b/Highly_likely_Table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3072505C-59BF-4732-A4BC-8722560F3C6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27A6A62-DC00-4466-973A-0E2C2ABFB6CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Cat</t>
   </si>
@@ -71,6 +71,18 @@
   </si>
   <si>
     <t>Satisfied</t>
+  </si>
+  <si>
+    <t>Chickcen</t>
+  </si>
+  <si>
+    <t>Rat</t>
+  </si>
+  <si>
+    <t>Worry</t>
+  </si>
+  <si>
+    <t>Clever</t>
   </si>
 </sst>
 </file>
@@ -399,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -495,6 +507,28 @@
         <v>16</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
In HL excel cells became partialy red
</commit_message>
<xml_diff>
--- a/Highly_likely_Table.xlsx
+++ b/Highly_likely_Table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27A6A62-DC00-4466-973A-0E2C2ABFB6CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D74A47C-C08A-42EB-93A5-7C88FA40E5AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Cat</t>
   </si>
@@ -83,13 +83,16 @@
   </si>
   <si>
     <t>Clever</t>
+  </si>
+  <si>
+    <t>In master branch it became RED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +104,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -126,11 +136,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,15 +422,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -430,18 +441,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -452,7 +466,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -463,7 +477,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -474,7 +488,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -485,7 +499,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -496,7 +510,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -507,7 +521,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -518,7 +532,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Revert "Green in excel"
This reverts commit 70cdc587446050a292d128816348821ecbcdcc21.
</commit_message>
<xml_diff>
--- a/Highly_likely_Table.xlsx
+++ b/Highly_likely_Table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2437D2-B334-4598-AE3B-336D6E70DFA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27A6A62-DC00-4466-973A-0E2C2ABFB6CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Cat</t>
   </si>
@@ -83,16 +83,13 @@
   </si>
   <si>
     <t>Clever</t>
-  </si>
-  <si>
-    <t>Green in testbranch00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,13 +101,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="9" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -136,12 +126,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,15 +411,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -441,7 +430,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -452,7 +441,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -463,7 +452,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -474,7 +463,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -485,7 +474,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -496,50 +485,47 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8">
         <v>10</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9">
         <v>3</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10">
         <v>2</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>